<commit_message>
Guarantor 10 test cases
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/3001-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-DISBURSE-FEE-%APR-AMT-Regular-CASH-Newcreateloan.xlsx
+++ b/Mifos Automation Excels/Client/3001-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-DISBURSE-FEE-%APR-AMT-Regular-CASH-Newcreateloan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mifosx-e2e-testing\Mifos Automation Excels\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -237,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,11 +383,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -431,7 +467,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -464,9 +500,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,6 +552,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1689,8 +1759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,8 +1858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>